<commit_message>
Added Dashboard test cases
</commit_message>
<xml_diff>
--- a/TestData/IMI_Automation_TestData.xlsx
+++ b/TestData/IMI_Automation_TestData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Other_Details_TestData" sheetId="4" r:id="rId4"/>
+    <sheet name="g" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -539,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -718,4 +719,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>